<commit_message>
Actualizado y arreglado "Estado diario web"
</commit_message>
<xml_diff>
--- a/salida/datos_gid_134160.xlsx
+++ b/salida/datos_gid_134160.xlsx
@@ -160,8 +160,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:N64" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:N64"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:N65" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:N65"/>
   <tableColumns count="14">
     <tableColumn id="1" name="gid"/>
     <tableColumn id="2" name="Fecha"/>
@@ -532,7 +532,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45746</v>
+        <v>45748</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -551,18 +551,18 @@
         <v>18</v>
       </c>
       <c r="I2" t="n">
-        <v>3040379</v>
+        <v>3040714</v>
       </c>
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2" s="1" t="n">
-        <v>45746.9736111111</v>
+        <v>45749.0423611111</v>
       </c>
       <c r="M2" t="s">
         <v>19</v>
       </c>
       <c r="N2" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -570,7 +570,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -589,12 +589,12 @@
         <v>18</v>
       </c>
       <c r="I3" t="n">
-        <v>3039783</v>
+        <v>3040379</v>
       </c>
       <c r="J3"/>
       <c r="K3"/>
       <c r="L3" s="1" t="n">
-        <v>45743.9673611111</v>
+        <v>45746.9736111111</v>
       </c>
       <c r="M3" t="s">
         <v>19</v>
@@ -608,7 +608,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -627,12 +627,12 @@
         <v>18</v>
       </c>
       <c r="I4" t="n">
-        <v>3039227</v>
+        <v>3039783</v>
       </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4" s="1" t="n">
-        <v>45740.9763888889</v>
+        <v>45743.9673611111</v>
       </c>
       <c r="M4" t="s">
         <v>19</v>
@@ -646,7 +646,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -665,18 +665,18 @@
         <v>18</v>
       </c>
       <c r="I5" t="n">
-        <v>3038830</v>
+        <v>3039227</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5" s="1" t="n">
-        <v>45737.9791666667</v>
+        <v>45740.9763888889</v>
       </c>
       <c r="M5" t="s">
         <v>19</v>
       </c>
       <c r="N5" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6">
@@ -684,7 +684,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45735</v>
+        <v>45737</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -703,18 +703,18 @@
         <v>18</v>
       </c>
       <c r="I6" t="n">
-        <v>3038479</v>
+        <v>3038830</v>
       </c>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6" s="1" t="n">
-        <v>45735.9909722222</v>
+        <v>45737.9791666667</v>
       </c>
       <c r="M6" t="s">
         <v>19</v>
       </c>
       <c r="N6" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">
@@ -722,7 +722,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45732</v>
+        <v>45735</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -741,12 +741,12 @@
         <v>18</v>
       </c>
       <c r="I7" t="n">
-        <v>3037926</v>
+        <v>3038479</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7" s="1" t="n">
-        <v>45733.0201388889</v>
+        <v>45735.9909722222</v>
       </c>
       <c r="M7" t="s">
         <v>19</v>
@@ -760,7 +760,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45729</v>
+        <v>45732</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -779,18 +779,18 @@
         <v>18</v>
       </c>
       <c r="I8" t="n">
-        <v>3037557</v>
+        <v>3037926</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8" s="1" t="n">
-        <v>45729.9729166667</v>
+        <v>45733.0201388889</v>
       </c>
       <c r="M8" t="s">
         <v>19</v>
       </c>
       <c r="N8" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9">
@@ -798,7 +798,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45728</v>
+        <v>45729</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -817,22 +817,26 @@
         <v>18</v>
       </c>
       <c r="I9" t="n">
-        <v>3037348</v>
-      </c>
-      <c r="J9" t="s">
-        <v>20</v>
-      </c>
+        <v>3037557</v>
+      </c>
+      <c r="J9"/>
       <c r="K9"/>
-      <c r="L9" s="1"/>
-      <c r="M9"/>
-      <c r="N9"/>
+      <c r="L9" s="1" t="n">
+        <v>45729.9729166667</v>
+      </c>
+      <c r="M9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45727</v>
+        <v>45728</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -851,26 +855,22 @@
         <v>18</v>
       </c>
       <c r="I10" t="n">
-        <v>3037147</v>
-      </c>
-      <c r="J10"/>
+        <v>3037348</v>
+      </c>
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
       <c r="K10"/>
-      <c r="L10" s="1" t="n">
-        <v>45728.0736111111</v>
-      </c>
-      <c r="M10" t="s">
-        <v>19</v>
-      </c>
-      <c r="N10" t="n">
-        <v>100</v>
-      </c>
+      <c r="L10" s="1"/>
+      <c r="M10"/>
+      <c r="N10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45726</v>
+        <v>45727</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -889,22 +889,26 @@
         <v>18</v>
       </c>
       <c r="I11" t="n">
-        <v>3036911</v>
-      </c>
-      <c r="J11" t="s">
-        <v>20</v>
-      </c>
+        <v>3037147</v>
+      </c>
+      <c r="J11"/>
       <c r="K11"/>
-      <c r="L11" s="1"/>
-      <c r="M11"/>
-      <c r="N11"/>
+      <c r="L11" s="1" t="n">
+        <v>45728.0736111111</v>
+      </c>
+      <c r="M11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>45725</v>
+        <v>45726</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
@@ -923,10 +927,10 @@
         <v>18</v>
       </c>
       <c r="I12" t="n">
-        <v>3036752</v>
+        <v>3036911</v>
       </c>
       <c r="J12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K12"/>
       <c r="L12" s="1"/>
@@ -938,7 +942,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45722</v>
+        <v>45725</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -957,26 +961,22 @@
         <v>18</v>
       </c>
       <c r="I13" t="n">
-        <v>3036414</v>
-      </c>
-      <c r="J13"/>
+        <v>3036752</v>
+      </c>
+      <c r="J13" t="s">
+        <v>21</v>
+      </c>
       <c r="K13"/>
-      <c r="L13" s="1" t="n">
-        <v>45722.9680555556</v>
-      </c>
-      <c r="M13" t="s">
-        <v>19</v>
-      </c>
-      <c r="N13" t="n">
-        <v>75</v>
-      </c>
+      <c r="L13" s="1"/>
+      <c r="M13"/>
+      <c r="N13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45721</v>
+        <v>45722</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -995,22 +995,26 @@
         <v>18</v>
       </c>
       <c r="I14" t="n">
-        <v>3036242</v>
-      </c>
-      <c r="J14" t="s">
-        <v>20</v>
-      </c>
+        <v>3036414</v>
+      </c>
+      <c r="J14"/>
       <c r="K14"/>
-      <c r="L14" s="1"/>
-      <c r="M14"/>
-      <c r="N14"/>
+      <c r="L14" s="1" t="n">
+        <v>45722.9680555556</v>
+      </c>
+      <c r="M14" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45719</v>
+        <v>45721</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
@@ -1029,26 +1033,22 @@
         <v>18</v>
       </c>
       <c r="I15" t="n">
-        <v>3035846</v>
-      </c>
-      <c r="J15"/>
+        <v>3036242</v>
+      </c>
+      <c r="J15" t="s">
+        <v>20</v>
+      </c>
       <c r="K15"/>
-      <c r="L15" s="1" t="n">
-        <v>45719.9756944444</v>
-      </c>
-      <c r="M15" t="s">
-        <v>19</v>
-      </c>
-      <c r="N15" t="n">
-        <v>75</v>
-      </c>
+      <c r="L15" s="1"/>
+      <c r="M15"/>
+      <c r="N15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45715</v>
+        <v>45719</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
@@ -1067,20 +1067,18 @@
         <v>18</v>
       </c>
       <c r="I16" t="n">
-        <v>3035486</v>
+        <v>3035846</v>
       </c>
       <c r="J16"/>
-      <c r="K16" t="s">
-        <v>22</v>
-      </c>
+      <c r="K16"/>
       <c r="L16" s="1" t="n">
-        <v>45716.1729166667</v>
+        <v>45719.9756944444</v>
       </c>
       <c r="M16" t="s">
         <v>19</v>
       </c>
       <c r="N16" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
@@ -1088,7 +1086,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45714</v>
+        <v>45715</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -1107,22 +1105,28 @@
         <v>18</v>
       </c>
       <c r="I17" t="n">
-        <v>3035307</v>
-      </c>
-      <c r="J17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17"/>
-      <c r="L17" s="1"/>
-      <c r="M17"/>
-      <c r="N17"/>
+        <v>3035486</v>
+      </c>
+      <c r="J17"/>
+      <c r="K17" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="1" t="n">
+        <v>45716.1729166667</v>
+      </c>
+      <c r="M17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45711</v>
+        <v>45714</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
@@ -1141,28 +1145,22 @@
         <v>18</v>
       </c>
       <c r="I18" t="n">
-        <v>3034751</v>
-      </c>
-      <c r="J18"/>
-      <c r="K18" t="s">
-        <v>24</v>
-      </c>
-      <c r="L18" s="1" t="n">
-        <v>45712.05</v>
-      </c>
-      <c r="M18" t="s">
-        <v>19</v>
-      </c>
-      <c r="N18" t="n">
-        <v>100</v>
-      </c>
+        <v>3035307</v>
+      </c>
+      <c r="J18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18"/>
+      <c r="L18" s="1"/>
+      <c r="M18"/>
+      <c r="N18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>45708</v>
+        <v>45711</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
@@ -1181,18 +1179,20 @@
         <v>18</v>
       </c>
       <c r="I19" t="n">
-        <v>3034350</v>
+        <v>3034751</v>
       </c>
       <c r="J19"/>
-      <c r="K19"/>
+      <c r="K19" t="s">
+        <v>24</v>
+      </c>
       <c r="L19" s="1" t="n">
-        <v>45709.0395833333</v>
+        <v>45712.05</v>
       </c>
       <c r="M19" t="s">
         <v>19</v>
       </c>
       <c r="N19" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20">
@@ -1200,7 +1200,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>45706</v>
+        <v>45708</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
@@ -1219,12 +1219,12 @@
         <v>18</v>
       </c>
       <c r="I20" t="n">
-        <v>3034016</v>
+        <v>3034350</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20" s="1" t="n">
-        <v>45707.0180555556</v>
+        <v>45709.0395833333</v>
       </c>
       <c r="M20" t="s">
         <v>19</v>
@@ -1238,7 +1238,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>45704</v>
+        <v>45706</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
@@ -1257,18 +1257,18 @@
         <v>18</v>
       </c>
       <c r="I21" t="n">
-        <v>3033608</v>
+        <v>3034016</v>
       </c>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21" s="1" t="n">
-        <v>45704.9854166667</v>
+        <v>45707.0180555556</v>
       </c>
       <c r="M21" t="s">
         <v>19</v>
       </c>
       <c r="N21" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22">
@@ -1276,7 +1276,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>45701</v>
+        <v>45704</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>
@@ -1295,18 +1295,18 @@
         <v>18</v>
       </c>
       <c r="I22" t="n">
-        <v>3033244</v>
+        <v>3033608</v>
       </c>
       <c r="J22"/>
       <c r="K22"/>
       <c r="L22" s="1" t="n">
-        <v>45702.0006944444</v>
+        <v>45704.9854166667</v>
       </c>
       <c r="M22" t="s">
         <v>19</v>
       </c>
       <c r="N22" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23">
@@ -1314,7 +1314,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>45698</v>
+        <v>45701</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
@@ -1333,12 +1333,12 @@
         <v>18</v>
       </c>
       <c r="I23" t="n">
-        <v>3032687</v>
+        <v>3033244</v>
       </c>
       <c r="J23"/>
       <c r="K23"/>
       <c r="L23" s="1" t="n">
-        <v>45698.9770833333</v>
+        <v>45702.0006944444</v>
       </c>
       <c r="M23" t="s">
         <v>19</v>
@@ -1352,7 +1352,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>45694</v>
+        <v>45698</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
@@ -1371,12 +1371,12 @@
         <v>18</v>
       </c>
       <c r="I24" t="n">
-        <v>3032163</v>
+        <v>3032687</v>
       </c>
       <c r="J24"/>
       <c r="K24"/>
       <c r="L24" s="1" t="n">
-        <v>45695.0444444444</v>
+        <v>45698.9770833333</v>
       </c>
       <c r="M24" t="s">
         <v>19</v>
@@ -1390,7 +1390,7 @@
         <v>14</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>45691</v>
+        <v>45694</v>
       </c>
       <c r="C25" t="s">
         <v>15</v>
@@ -1409,18 +1409,18 @@
         <v>18</v>
       </c>
       <c r="I25" t="n">
-        <v>3031611</v>
+        <v>3032163</v>
       </c>
       <c r="J25"/>
       <c r="K25"/>
       <c r="L25" s="1" t="n">
-        <v>45691.9895833333</v>
+        <v>45695.0444444444</v>
       </c>
       <c r="M25" t="s">
         <v>19</v>
       </c>
       <c r="N25" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26">
@@ -1428,7 +1428,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>45688</v>
+        <v>45691</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
@@ -1447,12 +1447,12 @@
         <v>18</v>
       </c>
       <c r="I26" t="n">
-        <v>3031161</v>
+        <v>3031611</v>
       </c>
       <c r="J26"/>
       <c r="K26"/>
       <c r="L26" s="1" t="n">
-        <v>45688.9875</v>
+        <v>45691.9895833333</v>
       </c>
       <c r="M26" t="s">
         <v>19</v>
@@ -1466,7 +1466,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>45685</v>
+        <v>45688</v>
       </c>
       <c r="C27" t="s">
         <v>15</v>
@@ -1485,18 +1485,18 @@
         <v>18</v>
       </c>
       <c r="I27" t="n">
-        <v>3030620</v>
+        <v>3031161</v>
       </c>
       <c r="J27"/>
       <c r="K27"/>
       <c r="L27" s="1" t="n">
-        <v>45686.0784722222</v>
+        <v>45688.9875</v>
       </c>
       <c r="M27" t="s">
         <v>19</v>
       </c>
       <c r="N27" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28">
@@ -1504,7 +1504,7 @@
         <v>14</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>45683</v>
+        <v>45685</v>
       </c>
       <c r="C28" t="s">
         <v>15</v>
@@ -1513,7 +1513,7 @@
         <v>16</v>
       </c>
       <c r="E28" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F28" t="s">
         <v>17</v>
@@ -1523,18 +1523,18 @@
         <v>18</v>
       </c>
       <c r="I28" t="n">
-        <v>3030209</v>
+        <v>3030620</v>
       </c>
       <c r="J28"/>
       <c r="K28"/>
       <c r="L28" s="1" t="n">
-        <v>45683.9986111111</v>
+        <v>45686.0784722222</v>
       </c>
       <c r="M28" t="s">
         <v>19</v>
       </c>
       <c r="N28" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29">
@@ -1542,7 +1542,7 @@
         <v>14</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>45680</v>
+        <v>45683</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
@@ -1561,18 +1561,18 @@
         <v>18</v>
       </c>
       <c r="I29" t="n">
-        <v>3029788</v>
+        <v>3030209</v>
       </c>
       <c r="J29"/>
       <c r="K29"/>
       <c r="L29" s="1" t="n">
-        <v>45681.0166666667</v>
+        <v>45683.9986111111</v>
       </c>
       <c r="M29" t="s">
         <v>19</v>
       </c>
       <c r="N29" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30">
@@ -1580,7 +1580,7 @@
         <v>14</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>45677</v>
+        <v>45680</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
@@ -1599,12 +1599,12 @@
         <v>18</v>
       </c>
       <c r="I30" t="n">
-        <v>3029244</v>
+        <v>3029788</v>
       </c>
       <c r="J30"/>
       <c r="K30"/>
       <c r="L30" s="1" t="n">
-        <v>45677.9743055556</v>
+        <v>45681.0166666667</v>
       </c>
       <c r="M30" t="s">
         <v>19</v>
@@ -1618,7 +1618,7 @@
         <v>14</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>45674</v>
+        <v>45677</v>
       </c>
       <c r="C31" t="s">
         <v>15</v>
@@ -1637,18 +1637,18 @@
         <v>18</v>
       </c>
       <c r="I31" t="n">
-        <v>3028879</v>
+        <v>3029244</v>
       </c>
       <c r="J31"/>
       <c r="K31"/>
       <c r="L31" s="1" t="n">
-        <v>45674.975</v>
+        <v>45677.9743055556</v>
       </c>
       <c r="M31" t="s">
         <v>19</v>
       </c>
       <c r="N31" t="n">
-        <v>25</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32">
@@ -1656,7 +1656,7 @@
         <v>14</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>45672</v>
+        <v>45674</v>
       </c>
       <c r="C32" t="s">
         <v>15</v>
@@ -1675,18 +1675,18 @@
         <v>18</v>
       </c>
       <c r="I32" t="n">
-        <v>3009491</v>
+        <v>3028879</v>
       </c>
       <c r="J32"/>
       <c r="K32"/>
       <c r="L32" s="1" t="n">
-        <v>45673.0625</v>
+        <v>45674.975</v>
       </c>
       <c r="M32" t="s">
         <v>19</v>
       </c>
       <c r="N32" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33">
@@ -1694,7 +1694,7 @@
         <v>14</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>45670</v>
+        <v>45672</v>
       </c>
       <c r="C33" t="s">
         <v>15</v>
@@ -1713,18 +1713,18 @@
         <v>18</v>
       </c>
       <c r="I33" t="n">
-        <v>3009151</v>
+        <v>3009491</v>
       </c>
       <c r="J33"/>
       <c r="K33"/>
       <c r="L33" s="1" t="n">
-        <v>45671.0479166667</v>
+        <v>45673.0625</v>
       </c>
       <c r="M33" t="s">
         <v>19</v>
       </c>
       <c r="N33" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34">
@@ -1732,7 +1732,7 @@
         <v>14</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45667</v>
+        <v>45670</v>
       </c>
       <c r="C34" t="s">
         <v>15</v>
@@ -1751,12 +1751,12 @@
         <v>18</v>
       </c>
       <c r="I34" t="n">
-        <v>3008912</v>
+        <v>3009151</v>
       </c>
       <c r="J34"/>
       <c r="K34"/>
       <c r="L34" s="1" t="n">
-        <v>45667.9888888889</v>
+        <v>45671.0479166667</v>
       </c>
       <c r="M34" t="s">
         <v>19</v>
@@ -1770,7 +1770,7 @@
         <v>14</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>45665</v>
+        <v>45667</v>
       </c>
       <c r="C35" t="s">
         <v>15</v>
@@ -1789,12 +1789,12 @@
         <v>18</v>
       </c>
       <c r="I35" t="n">
-        <v>3008588</v>
+        <v>3008912</v>
       </c>
       <c r="J35"/>
       <c r="K35"/>
       <c r="L35" s="1" t="n">
-        <v>45665.9833333333</v>
+        <v>45667.9888888889</v>
       </c>
       <c r="M35" t="s">
         <v>19</v>
@@ -1808,7 +1808,7 @@
         <v>14</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>45662</v>
+        <v>45665</v>
       </c>
       <c r="C36" t="s">
         <v>15</v>
@@ -1827,12 +1827,12 @@
         <v>18</v>
       </c>
       <c r="I36" t="n">
-        <v>3008054</v>
+        <v>3008588</v>
       </c>
       <c r="J36"/>
       <c r="K36"/>
       <c r="L36" s="1" t="n">
-        <v>45663.0805555556</v>
+        <v>45665.9833333333</v>
       </c>
       <c r="M36" t="s">
         <v>19</v>
@@ -1846,7 +1846,7 @@
         <v>14</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>45659</v>
+        <v>45662</v>
       </c>
       <c r="C37" t="s">
         <v>15</v>
@@ -1865,20 +1865,18 @@
         <v>18</v>
       </c>
       <c r="I37" t="n">
-        <v>3007611</v>
+        <v>3008054</v>
       </c>
       <c r="J37"/>
-      <c r="K37" t="s">
-        <v>25</v>
-      </c>
+      <c r="K37"/>
       <c r="L37" s="1" t="n">
-        <v>45660.0881944444</v>
+        <v>45663.0805555556</v>
       </c>
       <c r="M37" t="s">
         <v>19</v>
       </c>
       <c r="N37" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38">
@@ -1886,7 +1884,7 @@
         <v>14</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>45655</v>
+        <v>45659</v>
       </c>
       <c r="C38" t="s">
         <v>15</v>
@@ -1905,12 +1903,14 @@
         <v>18</v>
       </c>
       <c r="I38" t="n">
-        <v>3007128</v>
+        <v>3007611</v>
       </c>
       <c r="J38"/>
-      <c r="K38"/>
+      <c r="K38" t="s">
+        <v>25</v>
+      </c>
       <c r="L38" s="1" t="n">
-        <v>45655.9923611111</v>
+        <v>45660.0881944444</v>
       </c>
       <c r="M38" t="s">
         <v>19</v>
@@ -1924,7 +1924,7 @@
         <v>14</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>45653</v>
+        <v>45655</v>
       </c>
       <c r="C39" t="s">
         <v>15</v>
@@ -1943,18 +1943,18 @@
         <v>18</v>
       </c>
       <c r="I39" t="n">
-        <v>3006827</v>
+        <v>3007128</v>
       </c>
       <c r="J39"/>
       <c r="K39"/>
       <c r="L39" s="1" t="n">
-        <v>45654.0194444444</v>
+        <v>45655.9923611111</v>
       </c>
       <c r="M39" t="s">
         <v>19</v>
       </c>
       <c r="N39" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40">
@@ -1962,7 +1962,7 @@
         <v>14</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>45650</v>
+        <v>45653</v>
       </c>
       <c r="C40" t="s">
         <v>15</v>
@@ -1978,15 +1978,15 @@
       </c>
       <c r="G40"/>
       <c r="H40" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="I40" t="n">
-        <v>3006321</v>
+        <v>3006827</v>
       </c>
       <c r="J40"/>
       <c r="K40"/>
       <c r="L40" s="1" t="n">
-        <v>45650.5805555556</v>
+        <v>45654.0194444444</v>
       </c>
       <c r="M40" t="s">
         <v>19</v>
@@ -2000,7 +2000,7 @@
         <v>14</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>45647</v>
+        <v>45650</v>
       </c>
       <c r="C41" t="s">
         <v>15</v>
@@ -2016,21 +2016,21 @@
       </c>
       <c r="G41"/>
       <c r="H41" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I41" t="n">
-        <v>3005877</v>
+        <v>3006321</v>
       </c>
       <c r="J41"/>
       <c r="K41"/>
       <c r="L41" s="1" t="n">
-        <v>45648.0347222222</v>
+        <v>45650.5805555556</v>
       </c>
       <c r="M41" t="s">
         <v>19</v>
       </c>
       <c r="N41" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42">
@@ -2038,7 +2038,7 @@
         <v>14</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>45643</v>
+        <v>45647</v>
       </c>
       <c r="C42" t="s">
         <v>15</v>
@@ -2057,14 +2057,12 @@
         <v>18</v>
       </c>
       <c r="I42" t="n">
-        <v>3004669</v>
+        <v>3005877</v>
       </c>
       <c r="J42"/>
-      <c r="K42" t="s">
-        <v>24</v>
-      </c>
+      <c r="K42"/>
       <c r="L42" s="1" t="n">
-        <v>45644.0131944444</v>
+        <v>45648.0347222222</v>
       </c>
       <c r="M42" t="s">
         <v>19</v>
@@ -2078,7 +2076,7 @@
         <v>14</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>45639</v>
+        <v>45643</v>
       </c>
       <c r="C43" t="s">
         <v>15</v>
@@ -2094,15 +2092,17 @@
       </c>
       <c r="G43"/>
       <c r="H43" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="I43" t="n">
-        <v>3003955</v>
+        <v>3004669</v>
       </c>
       <c r="J43"/>
-      <c r="K43"/>
+      <c r="K43" t="s">
+        <v>24</v>
+      </c>
       <c r="L43" s="1" t="n">
-        <v>45639.6534722222</v>
+        <v>45644.0131944444</v>
       </c>
       <c r="M43" t="s">
         <v>19</v>
@@ -2116,7 +2116,7 @@
         <v>14</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>45634</v>
+        <v>45639</v>
       </c>
       <c r="C44" t="s">
         <v>15</v>
@@ -2132,15 +2132,15 @@
       </c>
       <c r="G44"/>
       <c r="H44" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I44" t="n">
-        <v>3002628</v>
+        <v>3003955</v>
       </c>
       <c r="J44"/>
       <c r="K44"/>
       <c r="L44" s="1" t="n">
-        <v>45634.9826388889</v>
+        <v>45639.6534722222</v>
       </c>
       <c r="M44" t="s">
         <v>19</v>
@@ -2154,7 +2154,7 @@
         <v>14</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>45630</v>
+        <v>45634</v>
       </c>
       <c r="C45" t="s">
         <v>15</v>
@@ -2173,18 +2173,18 @@
         <v>18</v>
       </c>
       <c r="I45" t="n">
-        <v>3002035</v>
+        <v>3002628</v>
       </c>
       <c r="J45"/>
       <c r="K45"/>
       <c r="L45" s="1" t="n">
-        <v>45630.9972222222</v>
+        <v>45634.9826388889</v>
       </c>
       <c r="M45" t="s">
         <v>19</v>
       </c>
       <c r="N45" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46">
@@ -2192,7 +2192,7 @@
         <v>14</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>45627</v>
+        <v>45630</v>
       </c>
       <c r="C46" t="s">
         <v>15</v>
@@ -2208,21 +2208,21 @@
       </c>
       <c r="G46"/>
       <c r="H46" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="I46" t="n">
-        <v>3001402</v>
+        <v>3002035</v>
       </c>
       <c r="J46"/>
       <c r="K46"/>
       <c r="L46" s="1" t="n">
-        <v>45627.4541666667</v>
+        <v>45630.9972222222</v>
       </c>
       <c r="M46" t="s">
         <v>19</v>
       </c>
       <c r="N46" t="n">
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47">
@@ -2230,7 +2230,7 @@
         <v>14</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>45625</v>
+        <v>45627</v>
       </c>
       <c r="C47" t="s">
         <v>15</v>
@@ -2246,23 +2246,21 @@
       </c>
       <c r="G47"/>
       <c r="H47" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="I47" t="n">
-        <v>2999375</v>
+        <v>3001402</v>
       </c>
       <c r="J47"/>
-      <c r="K47" t="s">
-        <v>28</v>
-      </c>
+      <c r="K47"/>
       <c r="L47" s="1" t="n">
-        <v>45626.0479166667</v>
+        <v>45627.4541666667</v>
       </c>
       <c r="M47" t="s">
         <v>19</v>
       </c>
       <c r="N47" t="n">
-        <v>100</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48">
@@ -2270,7 +2268,7 @@
         <v>14</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>45622</v>
+        <v>45625</v>
       </c>
       <c r="C48" t="s">
         <v>15</v>
@@ -2289,18 +2287,20 @@
         <v>18</v>
       </c>
       <c r="I48" t="n">
-        <v>2984944</v>
+        <v>2999375</v>
       </c>
       <c r="J48"/>
-      <c r="K48"/>
+      <c r="K48" t="s">
+        <v>28</v>
+      </c>
       <c r="L48" s="1" t="n">
-        <v>45622.9979166667</v>
+        <v>45626.0479166667</v>
       </c>
       <c r="M48" t="s">
         <v>19</v>
       </c>
       <c r="N48" t="n">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49">
@@ -2308,7 +2308,7 @@
         <v>14</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>45610</v>
+        <v>45622</v>
       </c>
       <c r="C49" t="s">
         <v>15</v>
@@ -2317,7 +2317,7 @@
         <v>16</v>
       </c>
       <c r="E49" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F49" t="s">
         <v>17</v>
@@ -2327,12 +2327,12 @@
         <v>18</v>
       </c>
       <c r="I49" t="n">
-        <v>2949695</v>
+        <v>2984944</v>
       </c>
       <c r="J49"/>
       <c r="K49"/>
       <c r="L49" s="1" t="n">
-        <v>45610.9784722222</v>
+        <v>45622.9979166667</v>
       </c>
       <c r="M49" t="s">
         <v>19</v>
@@ -2346,7 +2346,7 @@
         <v>14</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>45607</v>
+        <v>45610</v>
       </c>
       <c r="C50" t="s">
         <v>15</v>
@@ -2365,12 +2365,12 @@
         <v>18</v>
       </c>
       <c r="I50" t="n">
-        <v>2949173</v>
+        <v>2949695</v>
       </c>
       <c r="J50"/>
       <c r="K50"/>
       <c r="L50" s="1" t="n">
-        <v>45607.9875</v>
+        <v>45610.9784722222</v>
       </c>
       <c r="M50" t="s">
         <v>19</v>
@@ -2384,7 +2384,7 @@
         <v>14</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>45603</v>
+        <v>45607</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
@@ -2403,18 +2403,18 @@
         <v>18</v>
       </c>
       <c r="I51" t="n">
-        <v>2948616</v>
+        <v>2949173</v>
       </c>
       <c r="J51"/>
       <c r="K51"/>
       <c r="L51" s="1" t="n">
-        <v>45603.9805555556</v>
+        <v>45607.9875</v>
       </c>
       <c r="M51" t="s">
         <v>19</v>
       </c>
       <c r="N51" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52">
@@ -2422,7 +2422,7 @@
         <v>14</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>45600</v>
+        <v>45603</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
@@ -2441,20 +2441,18 @@
         <v>18</v>
       </c>
       <c r="I52" t="n">
-        <v>2948153</v>
+        <v>2948616</v>
       </c>
       <c r="J52"/>
-      <c r="K52" t="s">
-        <v>22</v>
-      </c>
+      <c r="K52"/>
       <c r="L52" s="1" t="n">
-        <v>45600.9881944444</v>
+        <v>45603.9805555556</v>
       </c>
       <c r="M52" t="s">
         <v>19</v>
       </c>
       <c r="N52" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53">
@@ -2462,7 +2460,7 @@
         <v>14</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>45597</v>
+        <v>45600</v>
       </c>
       <c r="C53" t="s">
         <v>15</v>
@@ -2481,18 +2479,20 @@
         <v>18</v>
       </c>
       <c r="I53" t="n">
-        <v>2947810</v>
+        <v>2948153</v>
       </c>
       <c r="J53"/>
-      <c r="K53"/>
+      <c r="K53" t="s">
+        <v>22</v>
+      </c>
       <c r="L53" s="1" t="n">
-        <v>45597.9791666667</v>
+        <v>45600.9881944444</v>
       </c>
       <c r="M53" t="s">
         <v>19</v>
       </c>
       <c r="N53" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54">
@@ -2500,7 +2500,7 @@
         <v>14</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>45595</v>
+        <v>45597</v>
       </c>
       <c r="C54" t="s">
         <v>15</v>
@@ -2519,20 +2519,18 @@
         <v>18</v>
       </c>
       <c r="I54" t="n">
-        <v>2947457</v>
+        <v>2947810</v>
       </c>
       <c r="J54"/>
-      <c r="K54" t="s">
-        <v>29</v>
-      </c>
+      <c r="K54"/>
       <c r="L54" s="1" t="n">
-        <v>45595.9840277778</v>
+        <v>45597.9791666667</v>
       </c>
       <c r="M54" t="s">
         <v>19</v>
       </c>
       <c r="N54" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55">
@@ -2540,7 +2538,7 @@
         <v>14</v>
       </c>
       <c r="B55" s="2" t="n">
-        <v>45593</v>
+        <v>45595</v>
       </c>
       <c r="C55" t="s">
         <v>15</v>
@@ -2559,12 +2557,14 @@
         <v>18</v>
       </c>
       <c r="I55" t="n">
-        <v>2947075</v>
+        <v>2947457</v>
       </c>
       <c r="J55"/>
-      <c r="K55"/>
+      <c r="K55" t="s">
+        <v>29</v>
+      </c>
       <c r="L55" s="1" t="n">
-        <v>45593.9736111111</v>
+        <v>45595.9840277778</v>
       </c>
       <c r="M55" t="s">
         <v>19</v>
@@ -2578,7 +2578,7 @@
         <v>14</v>
       </c>
       <c r="B56" s="2" t="n">
-        <v>45590</v>
+        <v>45593</v>
       </c>
       <c r="C56" t="s">
         <v>15</v>
@@ -2597,12 +2597,12 @@
         <v>18</v>
       </c>
       <c r="I56" t="n">
-        <v>2946703</v>
+        <v>2947075</v>
       </c>
       <c r="J56"/>
       <c r="K56"/>
       <c r="L56" s="1" t="n">
-        <v>45590.9826388889</v>
+        <v>45593.9736111111</v>
       </c>
       <c r="M56" t="s">
         <v>19</v>
@@ -2616,7 +2616,7 @@
         <v>14</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>45588</v>
+        <v>45590</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
@@ -2635,14 +2635,12 @@
         <v>18</v>
       </c>
       <c r="I57" t="n">
-        <v>2946330</v>
+        <v>2946703</v>
       </c>
       <c r="J57"/>
-      <c r="K57" t="s">
-        <v>25</v>
-      </c>
+      <c r="K57"/>
       <c r="L57" s="1" t="n">
-        <v>45588.9826388889</v>
+        <v>45590.9826388889</v>
       </c>
       <c r="M57" t="s">
         <v>19</v>
@@ -2656,7 +2654,7 @@
         <v>14</v>
       </c>
       <c r="B58" s="2" t="n">
-        <v>45585</v>
+        <v>45588</v>
       </c>
       <c r="C58" t="s">
         <v>15</v>
@@ -2675,14 +2673,14 @@
         <v>18</v>
       </c>
       <c r="I58" t="n">
-        <v>2945816</v>
+        <v>2946330</v>
       </c>
       <c r="J58"/>
       <c r="K58" t="s">
         <v>25</v>
       </c>
       <c r="L58" s="1" t="n">
-        <v>45585.98125</v>
+        <v>45588.9826388889</v>
       </c>
       <c r="M58" t="s">
         <v>19</v>
@@ -2696,7 +2694,7 @@
         <v>14</v>
       </c>
       <c r="B59" s="2" t="n">
-        <v>45581</v>
+        <v>45585</v>
       </c>
       <c r="C59" t="s">
         <v>15</v>
@@ -2715,12 +2713,14 @@
         <v>18</v>
       </c>
       <c r="I59" t="n">
-        <v>2944960</v>
+        <v>2945816</v>
       </c>
       <c r="J59"/>
-      <c r="K59"/>
+      <c r="K59" t="s">
+        <v>25</v>
+      </c>
       <c r="L59" s="1" t="n">
-        <v>45582.1284722222</v>
+        <v>45585.98125</v>
       </c>
       <c r="M59" t="s">
         <v>19</v>
@@ -2734,7 +2734,7 @@
         <v>14</v>
       </c>
       <c r="B60" s="2" t="n">
-        <v>45579</v>
+        <v>45581</v>
       </c>
       <c r="C60" t="s">
         <v>15</v>
@@ -2753,18 +2753,18 @@
         <v>18</v>
       </c>
       <c r="I60" t="n">
-        <v>2944572</v>
+        <v>2944960</v>
       </c>
       <c r="J60"/>
       <c r="K60"/>
       <c r="L60" s="1" t="n">
-        <v>45579.9833333333</v>
+        <v>45582.1284722222</v>
       </c>
       <c r="M60" t="s">
         <v>19</v>
       </c>
       <c r="N60" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61">
@@ -2772,7 +2772,7 @@
         <v>14</v>
       </c>
       <c r="B61" s="2" t="n">
-        <v>45576</v>
+        <v>45579</v>
       </c>
       <c r="C61" t="s">
         <v>15</v>
@@ -2791,12 +2791,12 @@
         <v>18</v>
       </c>
       <c r="I61" t="n">
-        <v>2944112</v>
+        <v>2944572</v>
       </c>
       <c r="J61"/>
       <c r="K61"/>
       <c r="L61" s="1" t="n">
-        <v>45576.9604166667</v>
+        <v>45579.9833333333</v>
       </c>
       <c r="M61" t="s">
         <v>19</v>
@@ -2810,7 +2810,7 @@
         <v>14</v>
       </c>
       <c r="B62" s="2" t="n">
-        <v>45574</v>
+        <v>45576</v>
       </c>
       <c r="C62" t="s">
         <v>15</v>
@@ -2829,18 +2829,18 @@
         <v>18</v>
       </c>
       <c r="I62" t="n">
-        <v>2943687</v>
+        <v>2944112</v>
       </c>
       <c r="J62"/>
       <c r="K62"/>
       <c r="L62" s="1" t="n">
-        <v>45574.9756944444</v>
+        <v>45576.9604166667</v>
       </c>
       <c r="M62" t="s">
         <v>19</v>
       </c>
       <c r="N62" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63">
@@ -2848,7 +2848,7 @@
         <v>14</v>
       </c>
       <c r="B63" s="2" t="n">
-        <v>45571</v>
+        <v>45574</v>
       </c>
       <c r="C63" t="s">
         <v>15</v>
@@ -2867,18 +2867,18 @@
         <v>18</v>
       </c>
       <c r="I63" t="n">
-        <v>2942801</v>
+        <v>2943687</v>
       </c>
       <c r="J63"/>
       <c r="K63"/>
       <c r="L63" s="1" t="n">
-        <v>45571.9743055556</v>
+        <v>45574.9756944444</v>
       </c>
       <c r="M63" t="s">
         <v>19</v>
       </c>
       <c r="N63" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64">
@@ -2886,7 +2886,7 @@
         <v>14</v>
       </c>
       <c r="B64" s="2" t="n">
-        <v>45568</v>
+        <v>45571</v>
       </c>
       <c r="C64" t="s">
         <v>15</v>
@@ -2905,19 +2905,57 @@
         <v>18</v>
       </c>
       <c r="I64" t="n">
+        <v>2942801</v>
+      </c>
+      <c r="J64"/>
+      <c r="K64"/>
+      <c r="L64" s="1" t="n">
+        <v>45571.9743055556</v>
+      </c>
+      <c r="M64" t="s">
+        <v>19</v>
+      </c>
+      <c r="N64" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" s="2" t="n">
+        <v>45568</v>
+      </c>
+      <c r="C65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" t="n">
+        <v>16</v>
+      </c>
+      <c r="F65" t="s">
+        <v>17</v>
+      </c>
+      <c r="G65"/>
+      <c r="H65" t="s">
+        <v>18</v>
+      </c>
+      <c r="I65" t="n">
         <v>2942135</v>
       </c>
-      <c r="J64"/>
-      <c r="K64" t="s">
+      <c r="J65"/>
+      <c r="K65" t="s">
         <v>25</v>
       </c>
-      <c r="L64" s="1" t="n">
+      <c r="L65" s="1" t="n">
         <v>45568.9881944444</v>
       </c>
-      <c r="M64" t="s">
-        <v>19</v>
-      </c>
-      <c r="N64" t="n">
+      <c r="M65" t="s">
+        <v>19</v>
+      </c>
+      <c r="N65" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>